<commit_message>
new excel sheet (working properly)
</commit_message>
<xml_diff>
--- a/combined_data.xlsx
+++ b/combined_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,57 +434,40 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>so</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>maybe</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>